<commit_message>
syncing example docs between enterprise and community branches
</commit_message>
<xml_diff>
--- a/doc/user-guide/examples/demand/demand-priorities.xlsx
+++ b/doc/user-guide/examples/demand/demand-priorities.xlsx
@@ -1,36 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\frepple\community\doc\user-guide\cookbook\demand\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\frepple\enterprise\doc\user-guide\examples\demand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D39A23D-EBFB-4944-8734-EFBCC4DC590F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4268D0A8-84A0-445E-9939-B870CC902DC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="3396" windowWidth="17280" windowHeight="8964" tabRatio="777" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="777" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="buffer" sheetId="1" r:id="rId1"/>
-    <sheet name="calendar bucket" sheetId="2" r:id="rId2"/>
-    <sheet name="calendar" sheetId="3" r:id="rId3"/>
-    <sheet name="customer" sheetId="4" r:id="rId4"/>
-    <sheet name="demand" sheetId="5" r:id="rId5"/>
-    <sheet name="operationmaterial" sheetId="6" r:id="rId6"/>
-    <sheet name="item" sheetId="7" r:id="rId7"/>
-    <sheet name="operationresource" sheetId="8" r:id="rId8"/>
-    <sheet name="location" sheetId="9" r:id="rId9"/>
-    <sheet name="operation" sheetId="11" r:id="rId10"/>
-    <sheet name="resource" sheetId="13" r:id="rId11"/>
-    <sheet name="parameter" sheetId="19" r:id="rId12"/>
+    <sheet name="calendar bucket" sheetId="2" r:id="rId1"/>
+    <sheet name="calendar" sheetId="3" r:id="rId2"/>
+    <sheet name="customer" sheetId="4" r:id="rId3"/>
+    <sheet name="demand" sheetId="5" r:id="rId4"/>
+    <sheet name="operationmaterial" sheetId="6" r:id="rId5"/>
+    <sheet name="item" sheetId="7" r:id="rId6"/>
+    <sheet name="operationresource" sheetId="8" r:id="rId7"/>
+    <sheet name="location" sheetId="9" r:id="rId8"/>
+    <sheet name="operation" sheetId="11" r:id="rId9"/>
+    <sheet name="resource" sheetId="13" r:id="rId10"/>
+    <sheet name="parameter" sheetId="19" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="50">
   <si>
     <t>name</t>
   </si>
@@ -55,12 +55,6 @@
     <t>item</t>
   </si>
   <si>
-    <t>onhand</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
@@ -136,9 +130,6 @@
     <t>end</t>
   </si>
   <si>
-    <t>start</t>
-  </si>
-  <si>
     <t>resource</t>
   </si>
   <si>
@@ -151,9 +142,6 @@
     <t>duration per unit</t>
   </si>
   <si>
-    <t>fixed_time</t>
-  </si>
-  <si>
     <t>time_per</t>
   </si>
   <si>
@@ -188,9 +176,6 @@
   </si>
   <si>
     <t>factory</t>
-  </si>
-  <si>
-    <t>Ship product</t>
   </si>
   <si>
     <t>Client 1</t>
@@ -579,41 +564,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
+        <v>21</v>
+      </c>
+      <c r="B2" s="1">
+        <v>36892</v>
+      </c>
+      <c r="C2" s="1">
+        <v>47848</v>
       </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0.70832175925925922</v>
       </c>
     </row>
   </sheetData>
@@ -622,81 +671,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2">
-        <f>8*3600</f>
-        <v>28800</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3">
-        <v>3600</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -719,10 +693,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -730,16 +704,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -747,12 +721,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,7 +741,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -775,35 +749,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1">
-        <v>41640</v>
+        <v>43831</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -812,113 +786,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="1">
-        <v>36892</v>
-      </c>
-      <c r="C2" s="1">
-        <v>47848</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0.375</v>
-      </c>
-      <c r="N2" s="2">
-        <v>0.70832175925925922</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -936,12 +803,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -952,7 +819,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -972,7 +839,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -980,12 +847,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,12 +868,12 @@
     <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -1015,43 +882,40 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>28</v>
-      </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>"Demand prio " &amp; H2 &amp; " due " &amp; TEXT(E2,"yyyy-mm-dd")</f>
-        <v>Demand prio 1 due 2013-12-06</v>
+        <v>Demand prio 1 due 2019-12-06</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E2" s="1">
-        <v>41614</v>
+        <v>43805</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -1062,29 +926,26 @@
       <c r="I2">
         <v>2</v>
       </c>
-      <c r="J2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A14" si="0">"Demand prio " &amp; H3 &amp; " due " &amp; TEXT(E3,"yyyy-mm-dd")</f>
-        <v>Demand prio 1 due 2013-12-20</v>
+        <v>Demand prio 1 due 2019-12-20</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1">
-        <v>41628</v>
+        <v>43819</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1095,29 +956,26 @@
       <c r="I3">
         <v>2</v>
       </c>
-      <c r="J3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>Demand prio 1 due 2014-01-01</v>
+        <v>Demand prio 1 due 2020-01-01</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E4" s="1">
-        <v>41640</v>
+        <v>43831</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -1128,29 +986,26 @@
       <c r="I4">
         <v>4</v>
       </c>
-      <c r="J4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>Demand prio 2 due 2013-12-30</v>
+        <v>Demand prio 2 due 2019-12-30</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E5" s="1">
-        <v>41638</v>
+        <v>43829</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G5">
         <v>6</v>
@@ -1161,29 +1016,26 @@
       <c r="I5">
         <v>6</v>
       </c>
-      <c r="J5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
-        <v>Demand prio 3 due 2013-12-29</v>
+        <v>Demand prio 3 due 2019-12-29</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E6" s="1">
-        <v>41637</v>
+        <v>43828</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -1194,29 +1046,26 @@
       <c r="I6">
         <v>5</v>
       </c>
-      <c r="J6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>Demand prio 1 due 2013-12-07</v>
+        <v>Demand prio 1 due 2019-12-07</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1">
-        <v>41615</v>
+        <v>43806</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G7">
         <v>5</v>
@@ -1227,29 +1076,26 @@
       <c r="I7">
         <v>5</v>
       </c>
-      <c r="J7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
-        <v>Demand prio 1 due 2013-12-31</v>
+        <v>Demand prio 1 due 2019-12-31</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E8" s="1">
-        <v>41639</v>
+        <v>43830</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G8">
         <v>9</v>
@@ -1260,29 +1106,26 @@
       <c r="I8">
         <v>9</v>
       </c>
-      <c r="J8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
-        <v>Demand prio 2 due 2013-12-09</v>
+        <v>Demand prio 2 due 2019-12-09</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E9" s="1">
-        <v>41617</v>
+        <v>43808</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1293,29 +1136,26 @@
       <c r="I9">
         <v>1</v>
       </c>
-      <c r="J9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>Demand prio 2 due 2013-12-17</v>
+        <v>Demand prio 2 due 2019-12-17</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E10" s="1">
-        <v>41625</v>
+        <v>43816</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>6</v>
@@ -1326,29 +1166,26 @@
       <c r="I10">
         <v>6</v>
       </c>
-      <c r="J10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>Demand prio 2 due 2013-12-17</v>
+        <v>Demand prio 2 due 2019-12-17</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1">
-        <v>41625</v>
+        <v>43816</v>
       </c>
       <c r="F11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G11">
         <v>9</v>
@@ -1359,29 +1196,26 @@
       <c r="I11">
         <v>9</v>
       </c>
-      <c r="J11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>Demand prio 1 due 2013-12-04</v>
+        <v>Demand prio 1 due 2019-12-04</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E12" s="1">
-        <v>41612</v>
+        <v>43803</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -1392,29 +1226,26 @@
       <c r="I12">
         <v>3</v>
       </c>
-      <c r="J12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>Demand prio 3 due 2013-12-11</v>
+        <v>Demand prio 3 due 2019-12-11</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E13" s="1">
-        <v>41619</v>
+        <v>43810</v>
       </c>
       <c r="F13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G13">
         <v>4</v>
@@ -1425,29 +1256,26 @@
       <c r="I13">
         <v>4</v>
       </c>
-      <c r="J13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
-        <v>Demand prio 3 due 2013-12-24</v>
+        <v>Demand prio 3 due 2019-12-24</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E14" s="1">
-        <v>41632</v>
+        <v>43823</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G14">
         <v>7</v>
@@ -1457,9 +1285,6 @@
       </c>
       <c r="I14">
         <v>7</v>
-      </c>
-      <c r="J14" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1467,12 +1292,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1485,13 +1310,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1499,30 +1324,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>-1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1530,7 +1341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1551,7 +1362,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1559,7 +1370,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1576,21 +1387,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1601,7 +1412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1620,15 +1431,72 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="2">
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>